<commit_message>
cambios en la base y diseño
</commit_message>
<xml_diff>
--- a/database/data/candidatos2023.xlsx
+++ b/database/data/candidatos2023.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dev-two\Documents\Proyectos\Control electoral\Documentos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\control_electoral\database\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{DAD16FB4-D7A0-470B-916D-2C341977A333}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD2F660E-4E76-4E04-A22A-7711F83E7E92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{700208B2-6CCD-4CD2-8160-51AA995EA349}"/>
   </bookViews>
@@ -27,7 +27,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -35,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
   <si>
     <t>N</t>
   </si>
@@ -46,91 +45,88 @@
     <t>Total de Votos</t>
   </si>
   <si>
-    <t>Candidato A</t>
-  </si>
-  <si>
     <t xml:space="preserve">Nombre del Partido </t>
   </si>
   <si>
     <t xml:space="preserve">Numero de Lista </t>
   </si>
   <si>
-    <t>Candidato B</t>
-  </si>
-  <si>
-    <t>Candidato C</t>
-  </si>
-  <si>
-    <t>Candidato D</t>
-  </si>
-  <si>
-    <t>Candidato E</t>
-  </si>
-  <si>
-    <t>Candidato F</t>
-  </si>
-  <si>
-    <t>Candidato G</t>
-  </si>
-  <si>
-    <t>Candidato H</t>
-  </si>
-  <si>
-    <t>Candidato I</t>
-  </si>
-  <si>
-    <t>PA</t>
-  </si>
-  <si>
-    <t>PB</t>
-  </si>
-  <si>
-    <t>PG</t>
-  </si>
-  <si>
-    <t>PH</t>
-  </si>
-  <si>
-    <t>PI</t>
-  </si>
-  <si>
-    <t>PC</t>
-  </si>
-  <si>
-    <t>PD</t>
-  </si>
-  <si>
-    <t>PE</t>
-  </si>
-  <si>
-    <t>PF</t>
-  </si>
-  <si>
-    <t>L1</t>
-  </si>
-  <si>
-    <t>L2</t>
-  </si>
-  <si>
-    <t>L3</t>
-  </si>
-  <si>
-    <t>L4</t>
-  </si>
-  <si>
-    <t>L5</t>
-  </si>
-  <si>
-    <t>L6</t>
-  </si>
-  <si>
-    <t>L7</t>
-  </si>
-  <si>
-    <t>L8</t>
-  </si>
-  <si>
-    <t>L9</t>
+    <t>Alianza Somos Agua</t>
+  </si>
+  <si>
+    <t>Sebastián Dávalos Sánchez</t>
+  </si>
+  <si>
+    <t>Xavier Vilcacundo Chamorro</t>
+  </si>
+  <si>
+    <t>Sociedad Patriótica</t>
+  </si>
+  <si>
+    <t>2-17</t>
+  </si>
+  <si>
+    <t>Felipe Bonilla López</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Alianza PSC-TC </t>
+  </si>
+  <si>
+    <t>6-61</t>
+  </si>
+  <si>
+    <t>Carlos Ortega Sevilla</t>
+  </si>
+  <si>
+    <t>Izquierda Demócratica</t>
+  </si>
+  <si>
+    <t>Myriam Auz Hidalgo</t>
+  </si>
+  <si>
+    <t>Alianza Clicc</t>
+  </si>
+  <si>
+    <t>16-20-100</t>
+  </si>
+  <si>
+    <t>Diana Caiza Telenchana</t>
+  </si>
+  <si>
+    <t>Pachakutik</t>
+  </si>
+  <si>
+    <t>18</t>
+  </si>
+  <si>
+    <t>12</t>
+  </si>
+  <si>
+    <t>Salomé Marín Núñez</t>
+  </si>
+  <si>
+    <t>Alianza Oportunidades</t>
+  </si>
+  <si>
+    <t>21-23-25-8</t>
+  </si>
+  <si>
+    <t>Luis Amoroso Mora</t>
+  </si>
+  <si>
+    <t>Reto</t>
+  </si>
+  <si>
+    <t>33</t>
+  </si>
+  <si>
+    <t>Javier Altamirano Sánchez</t>
+  </si>
+  <si>
+    <t>Solidariamente</t>
+  </si>
+  <si>
+    <t>63</t>
   </si>
 </sst>
 </file>
@@ -174,7 +170,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -186,6 +182,9 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -494,7 +493,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -505,14 +504,14 @@
   <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="4.7109375" customWidth="1"/>
-    <col min="2" max="2" width="26.85546875" customWidth="1"/>
-    <col min="3" max="3" width="22" customWidth="1"/>
+    <col min="2" max="2" width="47.85546875" customWidth="1"/>
+    <col min="3" max="3" width="36" customWidth="1"/>
     <col min="4" max="4" width="22.7109375" customWidth="1"/>
     <col min="5" max="5" width="13.7109375" customWidth="1"/>
   </cols>
@@ -525,10 +524,10 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>4</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>5</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>2</v>
@@ -539,13 +538,13 @@
         <v>1</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>23</v>
+        <v>5</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>9</v>
       </c>
       <c r="E2" s="2">
         <v>0</v>
@@ -556,13 +555,13 @@
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>24</v>
+        <v>8</v>
+      </c>
+      <c r="D3" s="2">
+        <v>3</v>
       </c>
       <c r="E3" s="2">
         <v>0</v>
@@ -573,13 +572,13 @@
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>25</v>
+        <v>11</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>12</v>
       </c>
       <c r="E4" s="2">
         <v>0</v>
@@ -590,13 +589,13 @@
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>26</v>
+        <v>14</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>21</v>
       </c>
       <c r="E5" s="2">
         <v>0</v>
@@ -607,13 +606,13 @@
         <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>27</v>
+        <v>16</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>17</v>
       </c>
       <c r="E6" s="2">
         <v>0</v>
@@ -624,13 +623,13 @@
         <v>6</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>28</v>
+        <v>19</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>20</v>
       </c>
       <c r="E7" s="2">
         <v>0</v>
@@ -641,13 +640,13 @@
         <v>7</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>11</v>
+        <v>22</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>29</v>
+        <v>23</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>24</v>
       </c>
       <c r="E8" s="2">
         <v>0</v>
@@ -658,13 +657,13 @@
         <v>8</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>12</v>
+        <v>25</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>30</v>
+        <v>26</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>27</v>
       </c>
       <c r="E9" s="2">
         <v>0</v>
@@ -675,13 +674,13 @@
         <v>9</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>13</v>
+        <v>28</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>30</v>
       </c>
       <c r="E10" s="2">
         <v>0</v>

</xml_diff>